<commit_message>
Included changes for callitspringurl
</commit_message>
<xml_diff>
--- a/Aldo-Test-Data.xlsx
+++ b/Aldo-Test-Data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hari4\aldo-webui-python-selenium\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hari4\python-webui-filter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86E39C75-5972-4636-90E5-E3EE4E6F79C3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FD8F3FA-9B4E-4842-B06E-F5DBEE485275}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{EDF5FB46-B36E-40B2-AB95-F94766D28BEB}"/>
+    <workbookView xWindow="4365" yWindow="4215" windowWidth="21600" windowHeight="11385" xr2:uid="{EDF5FB46-B36E-40B2-AB95-F94766D28BEB}"/>
   </bookViews>
   <sheets>
     <sheet name="Filter" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="27">
   <si>
     <t>https://www.aldoshoes.com</t>
   </si>
@@ -41,18 +41,12 @@
     <t>Women</t>
   </si>
   <si>
-    <t>Men</t>
-  </si>
-  <si>
     <t>Button</t>
   </si>
   <si>
     <t>Menu</t>
   </si>
   <si>
-    <t>New Arrivals</t>
-  </si>
-  <si>
     <t>Ankle boots</t>
   </si>
   <si>
@@ -71,9 +65,6 @@
     <t>filter_by</t>
   </si>
   <si>
-    <t>boots</t>
-  </si>
-  <si>
     <t>not applicable</t>
   </si>
   <si>
@@ -119,13 +110,7 @@
     <t>FilterbyMenuHover</t>
   </si>
   <si>
-    <t>FilterbyMenuClick</t>
-  </si>
-  <si>
     <t>FilterbyButton</t>
-  </si>
-  <si>
-    <t>FilterbyMenuMen</t>
   </si>
   <si>
     <t>Tote bags</t>
@@ -505,10 +490,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27055333-EC44-4601-BC90-7E0FD21D8139}">
-  <dimension ref="A1:L6"/>
+  <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:L5"/>
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -528,54 +513,54 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
         <v>9</v>
       </c>
-      <c r="B1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L1" t="s">
         <v>11</v>
-      </c>
-      <c r="D1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G1" t="s">
-        <v>23</v>
-      </c>
-      <c r="H1" t="s">
-        <v>16</v>
-      </c>
-      <c r="I1" t="s">
-        <v>24</v>
-      </c>
-      <c r="J1" t="s">
-        <v>25</v>
-      </c>
-      <c r="K1" t="s">
-        <v>26</v>
-      </c>
-      <c r="L1" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="E2" t="s">
         <v>1</v>
@@ -584,14 +569,14 @@
         <v>1</v>
       </c>
       <c r="G2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="I2" s="3"/>
       <c r="J2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="L2">
         <v>1</v>
@@ -599,120 +584,66 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F3" t="s">
         <v>1</v>
       </c>
       <c r="G3" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="I3">
         <v>5</v>
       </c>
       <c r="J3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="L3">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>30</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E4" t="s">
-        <v>5</v>
-      </c>
-      <c r="F4" t="s">
-        <v>2</v>
-      </c>
-      <c r="G4" t="s">
-        <v>17</v>
-      </c>
-      <c r="H4" t="s">
-        <v>12</v>
-      </c>
-      <c r="L4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>28</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E5" t="s">
-        <v>1</v>
-      </c>
-      <c r="F5" t="s">
-        <v>1</v>
-      </c>
-      <c r="G5" t="s">
-        <v>17</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="I5" s="3"/>
-      <c r="J5" t="s">
-        <v>7</v>
-      </c>
-      <c r="L5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1" xr:uid="{D6B559CD-72F8-49D1-BA36-BBA53474A8FC}"/>
-    <hyperlink ref="B4" r:id="rId2" xr:uid="{82BF4090-0034-4D5E-A514-3A24491E73BF}"/>
-    <hyperlink ref="B2" r:id="rId3" xr:uid="{03EB1BA5-03E9-4535-B05D-651036E95E39}"/>
-    <hyperlink ref="B5" r:id="rId4" xr:uid="{36AF369C-8813-45F1-A311-EB050CB8B2C0}"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{FB2E6CC7-D256-4FC1-8D5C-054A88DA7364}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{CDF30B1E-8D0F-4E2B-B4D4-310C9C1EEAAA}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId5"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId3"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F65BFE220852654A94B0E24FAB8D414F" ma:contentTypeVersion="8" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="bdacad30f1d04398aad8d480b298e327">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="b7a2423e-e457-463e-bb09-ea35f27c79d5" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d7967f50696128c4f60bd15feea58994" ns3:_="">
     <xsd:import namespace="b7a2423e-e457-463e-bb09-ea35f27c79d5"/>
@@ -882,22 +813,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{26CAAAA5-B919-4882-8B55-7BA28EC43444}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{04331AB7-27E2-427E-B974-CFD943DB3B3A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3FF27198-C35E-49FE-AC2C-C7F5925F492B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -913,21 +846,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{04331AB7-27E2-427E-B974-CFD943DB3B3A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{26CAAAA5-B919-4882-8B55-7BA28EC43444}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>